<commit_message>
adding se workday course analysis files
</commit_message>
<xml_diff>
--- a/se/faculty_dept.xlsx
+++ b/se/faculty_dept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohansharma/Desktop/se/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB51B0A6-888E-1C4F-A512-11BAC86C4BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7345F367-94D7-FE40-959B-50F12C55487B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{AC6FBD2C-B37A-D441-902D-9AB17BDCFD1A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{AC6FBD2C-B37A-D441-902D-9AB17BDCFD1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="83">
   <si>
     <t>Ali Yassine</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Donald Schlomer</t>
-  </si>
-  <si>
-    <t>ME-A</t>
   </si>
   <si>
     <t>Earl Sprague</t>
@@ -669,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A73BE3-5891-CA44-95C3-A77CB042E69F}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,13 +679,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -699,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -710,7 +707,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -721,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -732,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -743,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -754,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -765,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -776,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -787,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -795,653 +792,653 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
-        <v>32</v>
-      </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
         <v>47</v>
       </c>
-      <c r="B43" t="s">
-        <v>48</v>
-      </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B67" t="s">
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>

</xml_diff>